<commit_message>
setting with all data
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephan\Desktop\repos\Michaelis-Menten-Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B00EE5-6FE9-4AF4-9F02-1896750116D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8633DF7B-4B89-473F-BE90-43EBE82BC037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2663" yWindow="1823" windowWidth="15389" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -401,11 +401,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B17" si="0">$F$3*A3/($F$2+A3)</f>
-        <v>0.5</v>
+        <v>1.446</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -416,29 +415,26 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>2.6469999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4.6719999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1.142857142857143</v>
+        <v>7.7729999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -446,98 +442,63 @@
         <v>0.5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>11.432</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333335</v>
+        <v>18.792000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>23.913</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>1.4545454545454546</v>
+        <v>26.5505</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>0.9</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>29.311499999999999</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>1.5384615384615383</v>
+        <v>32.101500000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>1.1000000000000001</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1.5714285714285714</v>
+        <v>31.4345</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>1.2</v>
+        <v>7.5</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1.5999999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>1.3</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1.625</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>1.4</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1.6470588235294117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>1.5</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666665</v>
+        <v>37.161999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>